<commit_message>
rewrote input files as xlsx for easier manipulation by hand
</commit_message>
<xml_diff>
--- a/data/TestLocation/input_data/conventional_generators.xlsx
+++ b/data/TestLocation/input_data/conventional_generators.xlsx
@@ -1,38 +1,330 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestLocation/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="356" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBECFD4A-0F4F-4ADC-9313-FD213D7CC6B9}"/>
   <bookViews>
-    <workbookView xWindow="-9220" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3110" yWindow="-13170" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>CostReserveG</t>
+  </si>
+  <si>
+    <t>PMinG</t>
+  </si>
+  <si>
+    <t>PMaxG</t>
+  </si>
+  <si>
+    <t>PMatterG</t>
+  </si>
+  <si>
+    <t>GHGupstreamG</t>
+  </si>
+  <si>
+    <t>GHGOperationG</t>
+  </si>
+  <si>
+    <t>generator_name</t>
+  </si>
+  <si>
+    <t>g1_coal</t>
+  </si>
+  <si>
+    <t>g2_diesel</t>
+  </si>
+  <si>
+    <t>TechG</t>
+  </si>
+  <si>
+    <t>CostCapGyear2020</t>
+  </si>
+  <si>
+    <t>CostCapGyear2025</t>
+  </si>
+  <si>
+    <t>CostCapGyear2030</t>
+  </si>
+  <si>
+    <t>CostCapGyear2035</t>
+  </si>
+  <si>
+    <t>CostCapGyear2040</t>
+  </si>
+  <si>
+    <t>CostCapGyear2045</t>
+  </si>
+  <si>
+    <t>CostCapGyear2050</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2020</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2025</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2030</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2035</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2040</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2045</t>
+  </si>
+  <si>
+    <t>CostOperationVarGyear2050</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2020</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2025</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2030</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2035</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2040</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2045</t>
+  </si>
+  <si>
+    <t>CostOperationFixGyear2050</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2020</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2025</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2030</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2035</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2040</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2045</t>
+  </si>
+  <si>
+    <t>LifetimeGyear2050</t>
+  </si>
+  <si>
+    <t>For Diesel CostCap/CostOp/Lifetime: C. Breyer's study CHP Oil Heating data used efficiency 30% cost of diesel included in variable costs</t>
+  </si>
+  <si>
+    <t>For Coal: Efficieny 33% cost of fuel included in variable costs</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2020</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2025</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2030</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2035</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2040</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2045</t>
+  </si>
+  <si>
+    <t>PexistingGb1y2050</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2020</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2025</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2030</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2035</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2040</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2045</t>
+  </si>
+  <si>
+    <t>PexistingGb2y2050</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2020</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2025</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2030</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2035</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2040</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2045</t>
+  </si>
+  <si>
+    <t>PexistingGb3y2050</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2020</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2025</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2030</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2035</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2040</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2045</t>
+  </si>
+  <si>
+    <t>PexistingGb4y2050</t>
+  </si>
+  <si>
+    <t>Ram M. et al. Global Energy System based on 100% Renewable Energy – Power, Heat, Transport and Desalination Sectors. Study by Lappeenranta University of Technology and Energy Watch Group, Lappeenranta, Berlin, March 2019.</t>
+  </si>
+  <si>
+    <t>IRENA (2018), Renewable Power Generation Costs in 2017, International Renewable Energy Agency, Abu Dhabi.</t>
+  </si>
+  <si>
+    <t>(GHG)</t>
+  </si>
+  <si>
+    <t>Vasilis M. Fthenakis, Life Cycle Analysis of Photovoltaics: Strategic Technology Assessment (excerpt of A Comprehensive Guide to Solar Energy Systems)</t>
+  </si>
+  <si>
+    <t>Special Report of the Intergovernmental Panel on Climate Change, Renewable Energy Sources and Climate Change Mitigation, PIK,Intergovernmental Panel on Climate Change 2012</t>
+  </si>
+  <si>
+    <t>NREL, Life Cycle Assessment Harmonization</t>
+  </si>
+  <si>
+    <t>Sources: (techno-economic)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -43,7 +335,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -51,15 +343,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{A1C00199-A94A-454F-965C-6203F67DCAA5}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="1" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -337,12 +664,871 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:BI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="33" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="61" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:61" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AG1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH1" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ1" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="AK1" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL1" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="AM1" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="AN1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="AO1" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="AP1" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="AR1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="AS1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="AT1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="AU1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="AV1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="AX1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="AY1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="AZ1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="BA1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="BB1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="BC1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="BD1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="BE1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="BG1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="BH1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="BI1" s="20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1030.3030000000001</v>
+      </c>
+      <c r="F2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="I2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="K2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1500</v>
+      </c>
+      <c r="M2">
+        <v>23.332999999999998</v>
+      </c>
+      <c r="N2">
+        <v>25.454999999999998</v>
+      </c>
+      <c r="O2">
+        <v>27.879000000000001</v>
+      </c>
+      <c r="P2">
+        <v>30.908999999999999</v>
+      </c>
+      <c r="Q2">
+        <v>33.636000000000003</v>
+      </c>
+      <c r="R2">
+        <v>33.636000000000003</v>
+      </c>
+      <c r="S2">
+        <v>33.636000000000003</v>
+      </c>
+      <c r="T2" s="10">
+        <v>20</v>
+      </c>
+      <c r="U2" s="10">
+        <v>20</v>
+      </c>
+      <c r="V2" s="10">
+        <v>20</v>
+      </c>
+      <c r="W2" s="10">
+        <v>20</v>
+      </c>
+      <c r="X2" s="10">
+        <v>20</v>
+      </c>
+      <c r="Y2" s="10">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="10">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="2">
+        <v>850</v>
+      </c>
+      <c r="AI2" s="10">
+        <v>720</v>
+      </c>
+      <c r="AJ2" s="10">
+        <v>720</v>
+      </c>
+      <c r="AK2" s="10">
+        <v>720</v>
+      </c>
+      <c r="AL2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="10">
+        <v>884</v>
+      </c>
+      <c r="AP2" s="10">
+        <v>544</v>
+      </c>
+      <c r="AQ2" s="10">
+        <v>544</v>
+      </c>
+      <c r="AR2" s="10">
+        <v>272</v>
+      </c>
+      <c r="AS2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="10">
+        <v>760</v>
+      </c>
+      <c r="AW2" s="10">
+        <v>760</v>
+      </c>
+      <c r="AX2" s="10">
+        <v>456</v>
+      </c>
+      <c r="AY2" s="10">
+        <v>152</v>
+      </c>
+      <c r="AZ2" s="10">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="10">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="10">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="8">
+        <v>3045.6390000000001</v>
+      </c>
+      <c r="BD2" s="8">
+        <v>2872.6390000000001</v>
+      </c>
+      <c r="BE2" s="7">
+        <v>1995.069</v>
+      </c>
+      <c r="BF2" s="7">
+        <v>1383.1690000000001</v>
+      </c>
+      <c r="BG2" s="7">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="7">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>833.33299999999997</v>
+      </c>
+      <c r="F3" s="10">
+        <v>880</v>
+      </c>
+      <c r="G3" s="10">
+        <v>880</v>
+      </c>
+      <c r="H3" s="10">
+        <v>880</v>
+      </c>
+      <c r="I3" s="10">
+        <v>880</v>
+      </c>
+      <c r="J3" s="10">
+        <v>880</v>
+      </c>
+      <c r="K3" s="10">
+        <v>880</v>
+      </c>
+      <c r="L3" s="10">
+        <v>880</v>
+      </c>
+      <c r="M3">
+        <v>117.333</v>
+      </c>
+      <c r="N3">
+        <v>132.667</v>
+      </c>
+      <c r="O3" s="10">
+        <v>148</v>
+      </c>
+      <c r="P3">
+        <v>146.333</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>145</v>
+      </c>
+      <c r="R3" s="10">
+        <v>145</v>
+      </c>
+      <c r="S3" s="10">
+        <v>145</v>
+      </c>
+      <c r="T3">
+        <v>74.8</v>
+      </c>
+      <c r="U3">
+        <v>74.8</v>
+      </c>
+      <c r="V3">
+        <v>74.8</v>
+      </c>
+      <c r="W3">
+        <v>74.8</v>
+      </c>
+      <c r="X3">
+        <v>74.8</v>
+      </c>
+      <c r="Y3">
+        <v>74.8</v>
+      </c>
+      <c r="Z3">
+        <v>74.8</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>30</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>1083</v>
+      </c>
+      <c r="AI3" s="10">
+        <v>1077</v>
+      </c>
+      <c r="AJ3" s="10">
+        <v>1074</v>
+      </c>
+      <c r="AK3" s="10">
+        <v>948</v>
+      </c>
+      <c r="AL3" s="10">
+        <v>331</v>
+      </c>
+      <c r="AM3" s="10">
+        <v>165</v>
+      </c>
+      <c r="AN3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="19">
+        <v>935.18367999999998</v>
+      </c>
+      <c r="AP3" s="19">
+        <v>800.88468</v>
+      </c>
+      <c r="AQ3" s="19">
+        <v>800.88468</v>
+      </c>
+      <c r="AR3" s="19">
+        <v>675.46468000000004</v>
+      </c>
+      <c r="AS3" s="8">
+        <v>81.8</v>
+      </c>
+      <c r="AT3" s="8">
+        <v>77.234999999999999</v>
+      </c>
+      <c r="AU3" s="10">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="8">
+        <v>1366.8796500000001</v>
+      </c>
+      <c r="AW3" s="8">
+        <v>1286.51955</v>
+      </c>
+      <c r="AX3" s="8">
+        <v>1286.51955</v>
+      </c>
+      <c r="AY3" s="8">
+        <v>1286.51955</v>
+      </c>
+      <c r="AZ3" s="8">
+        <v>539.43700000000001</v>
+      </c>
+      <c r="BA3" s="8">
+        <v>532.06700000000001</v>
+      </c>
+      <c r="BB3" s="9">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="7">
+        <v>267.77357999999998</v>
+      </c>
+      <c r="BD3" s="7">
+        <v>169.41273000000001</v>
+      </c>
+      <c r="BE3" s="7">
+        <v>161.41273000000001</v>
+      </c>
+      <c r="BF3" s="7">
+        <v>161.41273000000001</v>
+      </c>
+      <c r="BG3" s="7">
+        <v>49.031469999999999</v>
+      </c>
+      <c r="BH3" s="7">
+        <v>43.574869999999997</v>
+      </c>
+      <c r="BI3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="1"/>
+    </row>
+    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="16"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="10">
+        <v>200</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
unified column names with year-dependency
</commit_message>
<xml_diff>
--- a/data/TestLocation/input_data/conventional_generators.xlsx
+++ b/data/TestLocation/input_data/conventional_generators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestLocation/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="356" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBECFD4A-0F4F-4ADC-9313-FD213D7CC6B9}"/>
+  <xr:revisionPtr revIDLastSave="384" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29B3B2C-138F-48F7-9DC4-0B754E16270F}"/>
   <bookViews>
-    <workbookView xWindow="3110" yWindow="-13170" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4590" yWindow="-4740" windowWidth="20740" windowHeight="10750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -76,90 +76,6 @@
     <t>TechG</t>
   </si>
   <si>
-    <t>CostCapGyear2020</t>
-  </si>
-  <si>
-    <t>CostCapGyear2025</t>
-  </si>
-  <si>
-    <t>CostCapGyear2030</t>
-  </si>
-  <si>
-    <t>CostCapGyear2035</t>
-  </si>
-  <si>
-    <t>CostCapGyear2040</t>
-  </si>
-  <si>
-    <t>CostCapGyear2045</t>
-  </si>
-  <si>
-    <t>CostCapGyear2050</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2020</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2025</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2030</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2035</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2040</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2045</t>
-  </si>
-  <si>
-    <t>CostOperationVarGyear2050</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2020</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2025</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2030</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2035</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2040</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2045</t>
-  </si>
-  <si>
-    <t>CostOperationFixGyear2050</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2020</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2025</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2030</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2035</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2040</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2045</t>
-  </si>
-  <si>
-    <t>LifetimeGyear2050</t>
-  </si>
-  <si>
     <t>For Diesel CostCap/CostOp/Lifetime: C. Breyer's study CHP Oil Heating data used efficiency 30% cost of diesel included in variable costs</t>
   </si>
   <si>
@@ -269,6 +185,90 @@
   </si>
   <si>
     <t>Sources: (techno-economic)</t>
+  </si>
+  <si>
+    <t>CostCapGy2020</t>
+  </si>
+  <si>
+    <t>CostCapGy2025</t>
+  </si>
+  <si>
+    <t>CostCapGy2030</t>
+  </si>
+  <si>
+    <t>CostCapGy2035</t>
+  </si>
+  <si>
+    <t>CostCapGy2040</t>
+  </si>
+  <si>
+    <t>CostCapGy2045</t>
+  </si>
+  <si>
+    <t>CostCapGy2050</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2020</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2025</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2030</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2035</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2040</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2045</t>
+  </si>
+  <si>
+    <t>CostOperationVarGy2050</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2020</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2025</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2030</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2035</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2040</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2045</t>
+  </si>
+  <si>
+    <t>CostOperationFixGy2050</t>
+  </si>
+  <si>
+    <t>LifetimeGy2020</t>
+  </si>
+  <si>
+    <t>LifetimeGy2025</t>
+  </si>
+  <si>
+    <t>LifetimeGy2030</t>
+  </si>
+  <si>
+    <t>LifetimeGy2035</t>
+  </si>
+  <si>
+    <t>LifetimeGy2040</t>
+  </si>
+  <si>
+    <t>LifetimeGy2045</t>
+  </si>
+  <si>
+    <t>LifetimeGy2050</t>
   </si>
 </sst>
 </file>
@@ -666,8 +666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -703,172 +703,172 @@
         <v>8</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="G1" s="20" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="H1" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG1" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="AI1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="AJ1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="AK1" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="AL1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="AM1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="AN1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="AO1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="AP1" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="AQ1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="AR1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="AS1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="AT1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="AU1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="AV1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="AW1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="AX1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="AY1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AZ1" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="BA1" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="BB1" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="BC1" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="20" t="s">
+      <c r="BD1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="BE1" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="BF1" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="BG1" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="AH1" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI1" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ1" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="AK1" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="AL1" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM1" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="AN1" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="AO1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="AP1" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="AS1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="AT1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="AU1" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="AV1" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="AW1" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="AX1" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="AY1" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="AZ1" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="BA1" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="BB1" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="BC1" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="BD1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="BE1" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="BF1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="BG1" s="20" t="s">
-        <v>68</v>
-      </c>
       <c r="BH1" s="20" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="BI1" s="20" t="s">
-        <v>70</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
     </row>
     <row r="6" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="13"/>
@@ -1335,7 +1335,7 @@
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B7" s="14"/>
       <c r="C7" s="13"/>
@@ -1495,37 +1495,37 @@
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data files, remove redundant old versions
</commit_message>
<xml_diff>
--- a/data/TestLocation/input_data/conventional_generators.xlsx
+++ b/data/TestLocation/input_data/conventional_generators.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/70b0e526faaa1b23/Dokumente/Alles zum Studium/Master/Masterarbeit/Leelo/data/TestLocation/input_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="384" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29B3B2C-138F-48F7-9DC4-0B754E16270F}"/>
+  <xr:revisionPtr revIDLastSave="385" documentId="11_AD4DB114E441178AC67DF47F8ED2CE42693EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4AA6B5A-4256-4113-91C3-49C7E63FD5B3}"/>
   <bookViews>
-    <workbookView xWindow="-4590" yWindow="-4740" windowWidth="20740" windowHeight="10750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2230" yWindow="-10740" windowWidth="17280" windowHeight="8960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Diesel</t>
   </si>
@@ -80,90 +80,6 @@
   </si>
   <si>
     <t>For Coal: Efficieny 33% cost of fuel included in variable costs</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2020</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2025</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2030</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2035</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2040</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2045</t>
-  </si>
-  <si>
-    <t>PexistingGb1y2050</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2020</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2025</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2030</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2035</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2040</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2045</t>
-  </si>
-  <si>
-    <t>PexistingGb2y2050</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2020</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2025</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2030</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2035</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2040</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2045</t>
-  </si>
-  <si>
-    <t>PexistingGb3y2050</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2020</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2025</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2030</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2035</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2040</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2045</t>
-  </si>
-  <si>
-    <t>PexistingGb4y2050</t>
   </si>
   <si>
     <t>Ram M. et al. Global Energy System based on 100% Renewable Energy – Power, Heat, Transport and Desalination Sectors. Study by Lappeenranta University of Technology and Energy Watch Group, Lappeenranta, Berlin, March 2019.</t>
@@ -275,13 +191,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -358,7 +272,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -366,9 +280,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -380,7 +291,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -664,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI20"/>
+  <dimension ref="A1:AG20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,229 +593,144 @@
     <col min="13" max="19" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="26" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="33" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="61" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:33" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="R1" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="S1" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="T1" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="V1" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="X1" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y1" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="Z1" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="AA1" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="AB1" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="AC1" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="AD1" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="AE1" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="AF1" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="AG1" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="AH1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="AI1" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="AJ1" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="AK1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="AL1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="AM1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN1" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO1" s="20" t="s">
+      <c r="F1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" s="20" t="s">
+      <c r="G1" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="AQ1" s="20" t="s">
+      <c r="H1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="AR1" s="20" t="s">
+      <c r="I1" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AS1" s="20" t="s">
+      <c r="J1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="AT1" s="20" t="s">
+      <c r="K1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="AU1" s="20" t="s">
+      <c r="L1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="AV1" s="20" t="s">
+      <c r="M1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" s="20" t="s">
+      <c r="N1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="AX1" s="20" t="s">
+      <c r="O1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="20" t="s">
+      <c r="P1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="AZ1" s="20" t="s">
+      <c r="Q1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="BA1" s="20" t="s">
+      <c r="R1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" s="20" t="s">
+      <c r="S1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" s="20" t="s">
+      <c r="T1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="BD1" s="20" t="s">
+      <c r="U1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="BE1" s="20" t="s">
+      <c r="V1" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="BF1" s="20" t="s">
+      <c r="W1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="BG1" s="20" t="s">
+      <c r="X1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" s="20" t="s">
+      <c r="Y1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="BI1" s="20" t="s">
+      <c r="Z1" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.3">
+      <c r="AA1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="7">
         <v>0</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="7">
         <v>0</v>
       </c>
       <c r="E2">
         <v>1030.3030000000001</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="7">
         <v>1500</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="7">
         <v>1500</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="7">
         <v>1500</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="7">
         <v>1500</v>
       </c>
-      <c r="J2" s="10">
+      <c r="J2" s="7">
         <v>1500</v>
       </c>
-      <c r="K2" s="10">
+      <c r="K2" s="7">
         <v>1500</v>
       </c>
-      <c r="L2" s="10">
+      <c r="L2" s="7">
         <v>1500</v>
       </c>
       <c r="M2">
@@ -929,25 +754,25 @@
       <c r="S2">
         <v>33.636000000000003</v>
       </c>
-      <c r="T2" s="10">
+      <c r="T2" s="7">
         <v>20</v>
       </c>
-      <c r="U2" s="10">
+      <c r="U2" s="7">
         <v>20</v>
       </c>
-      <c r="V2" s="10">
+      <c r="V2" s="7">
         <v>20</v>
       </c>
-      <c r="W2" s="10">
+      <c r="W2" s="7">
         <v>20</v>
       </c>
-      <c r="X2" s="10">
+      <c r="X2" s="7">
         <v>20</v>
       </c>
-      <c r="Y2" s="10">
+      <c r="Y2" s="7">
         <v>20</v>
       </c>
-      <c r="Z2" s="10">
+      <c r="Z2" s="7">
         <v>20</v>
       </c>
       <c r="AA2" s="1">
@@ -971,126 +796,42 @@
       <c r="AG2" s="1">
         <v>40</v>
       </c>
-      <c r="AH2" s="2">
-        <v>850</v>
-      </c>
-      <c r="AI2" s="10">
-        <v>720</v>
-      </c>
-      <c r="AJ2" s="10">
-        <v>720</v>
-      </c>
-      <c r="AK2" s="10">
-        <v>720</v>
-      </c>
-      <c r="AL2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="10">
-        <v>884</v>
-      </c>
-      <c r="AP2" s="10">
-        <v>544</v>
-      </c>
-      <c r="AQ2" s="10">
-        <v>544</v>
-      </c>
-      <c r="AR2" s="10">
-        <v>272</v>
-      </c>
-      <c r="AS2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="10">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="10">
-        <v>760</v>
-      </c>
-      <c r="AW2" s="10">
-        <v>760</v>
-      </c>
-      <c r="AX2" s="10">
-        <v>456</v>
-      </c>
-      <c r="AY2" s="10">
-        <v>152</v>
-      </c>
-      <c r="AZ2" s="10">
-        <v>0</v>
-      </c>
-      <c r="BA2" s="10">
-        <v>0</v>
-      </c>
-      <c r="BB2" s="10">
-        <v>0</v>
-      </c>
-      <c r="BC2" s="8">
-        <v>3045.6390000000001</v>
-      </c>
-      <c r="BD2" s="8">
-        <v>2872.6390000000001</v>
-      </c>
-      <c r="BE2" s="7">
-        <v>1995.069</v>
-      </c>
-      <c r="BF2" s="7">
-        <v>1383.1690000000001</v>
-      </c>
-      <c r="BG2" s="7">
-        <v>0</v>
-      </c>
-      <c r="BH2" s="7">
-        <v>0</v>
-      </c>
-      <c r="BI2" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <v>0</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="7">
         <v>0</v>
       </c>
       <c r="E3">
         <v>833.33299999999997</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="7">
         <v>880</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="7">
         <v>880</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="7">
         <v>880</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="7">
         <v>880</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="7">
         <v>880</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="7">
         <v>880</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>880</v>
       </c>
       <c r="M3">
@@ -1099,19 +840,19 @@
       <c r="N3">
         <v>132.667</v>
       </c>
-      <c r="O3" s="10">
+      <c r="O3" s="7">
         <v>148</v>
       </c>
       <c r="P3">
         <v>146.333</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="7">
         <v>145</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="7">
         <v>145</v>
       </c>
-      <c r="S3" s="10">
+      <c r="S3" s="7">
         <v>145</v>
       </c>
       <c r="T3">
@@ -1156,92 +897,8 @@
       <c r="AG3" s="1">
         <v>30</v>
       </c>
-      <c r="AH3" s="2">
-        <v>1083</v>
-      </c>
-      <c r="AI3" s="10">
-        <v>1077</v>
-      </c>
-      <c r="AJ3" s="10">
-        <v>1074</v>
-      </c>
-      <c r="AK3" s="10">
-        <v>948</v>
-      </c>
-      <c r="AL3" s="10">
-        <v>331</v>
-      </c>
-      <c r="AM3" s="10">
-        <v>165</v>
-      </c>
-      <c r="AN3" s="10">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="19">
-        <v>935.18367999999998</v>
-      </c>
-      <c r="AP3" s="19">
-        <v>800.88468</v>
-      </c>
-      <c r="AQ3" s="19">
-        <v>800.88468</v>
-      </c>
-      <c r="AR3" s="19">
-        <v>675.46468000000004</v>
-      </c>
-      <c r="AS3" s="8">
-        <v>81.8</v>
-      </c>
-      <c r="AT3" s="8">
-        <v>77.234999999999999</v>
-      </c>
-      <c r="AU3" s="10">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="8">
-        <v>1366.8796500000001</v>
-      </c>
-      <c r="AW3" s="8">
-        <v>1286.51955</v>
-      </c>
-      <c r="AX3" s="8">
-        <v>1286.51955</v>
-      </c>
-      <c r="AY3" s="8">
-        <v>1286.51955</v>
-      </c>
-      <c r="AZ3" s="8">
-        <v>539.43700000000001</v>
-      </c>
-      <c r="BA3" s="8">
-        <v>532.06700000000001</v>
-      </c>
-      <c r="BB3" s="9">
-        <v>0</v>
-      </c>
-      <c r="BC3" s="7">
-        <v>267.77357999999998</v>
-      </c>
-      <c r="BD3" s="7">
-        <v>169.41273000000001</v>
-      </c>
-      <c r="BE3" s="7">
-        <v>161.41273000000001</v>
-      </c>
-      <c r="BF3" s="7">
-        <v>161.41273000000001</v>
-      </c>
-      <c r="BG3" s="7">
-        <v>49.031469999999999</v>
-      </c>
-      <c r="BH3" s="7">
-        <v>43.574869999999997</v>
-      </c>
-      <c r="BI3" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
@@ -1269,19 +926,18 @@
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-    </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
       <c r="K5" s="2"/>
       <c r="L5" s="3"/>
       <c r="M5" s="4"/>
@@ -1299,21 +955,20 @@
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-    </row>
-    <row r="6" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
       <c r="K6" s="2"/>
       <c r="L6" s="3"/>
       <c r="M6" s="4"/>
@@ -1331,21 +986,20 @@
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-    </row>
-    <row r="7" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
       <c r="K7" s="2"/>
       <c r="L7" s="3"/>
       <c r="M7" s="4"/>
@@ -1357,13 +1011,13 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1380,29 +1034,29 @@
       <c r="T8" s="6"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="9"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1427,11 +1081,11 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>200</v>
       </c>
       <c r="C11">
@@ -1452,11 +1106,11 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="7">
         <v>0</v>
       </c>
       <c r="C12">
@@ -1477,7 +1131,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1493,39 +1147,39 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:61" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:61" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:61" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>